<commit_message>
added some auth and fixed OnAfterRenderAsync firing infinitely while a page is open. Also removed unneccesary files
</commit_message>
<xml_diff>
--- a/pyNeedBodies/games.xlsx
+++ b/pyNeedBodies/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>id</t>
   </si>
@@ -43,31 +43,22 @@
     <t>goalie list</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Chris Bolton</t>
+    <t>0</t>
   </si>
   <si>
     <t>Nic Bolton</t>
   </si>
   <si>
-    <t>WFCU Centre - Windsor Family Credit Union Centre</t>
+    <t>20230906</t>
+  </si>
+  <si>
+    <t>1000</t>
   </si>
   <si>
     <t>Prospects Athletics</t>
   </si>
   <si>
-    <t>0;4;</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>2;3;</t>
+    <t>0;</t>
   </si>
 </sst>
 </file>
@@ -425,7 +416,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,57 +456,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="C2">
-        <v>20231010</v>
-      </c>
-      <c r="D2">
-        <v>1900</v>
+      <c r="D2" t="s">
+        <v>12</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
       </c>
       <c r="F2">
-        <v>20</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
+        <v>5</v>
       </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>20230906</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3">
-        <v>4</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update design of add game form and fixed Program.cs
</commit_message>
<xml_diff>
--- a/pyNeedBodies/games.xlsx
+++ b/pyNeedBodies/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>id</t>
   </si>
@@ -46,16 +46,25 @@
     <t>0</t>
   </si>
   <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>Nic Bolton</t>
   </si>
   <si>
-    <t>20230906</t>
-  </si>
-  <si>
-    <t>1000</t>
+    <t>20230908</t>
+  </si>
+  <si>
+    <t>2000</t>
   </si>
   <si>
     <t>Prospects Athletics</t>
+  </si>
+  <si>
+    <t>Atlas Tube Recreation Centre</t>
+  </si>
+  <si>
+    <t>nan</t>
   </si>
   <si>
     <t>0;</t>
@@ -416,7 +425,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -456,25 +465,51 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
         <v>11</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="C2">
+        <v>20230906</v>
+      </c>
+      <c r="D2">
+        <v>1000</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
+      <c r="G2" t="s">
+        <v>16</v>
+      </c>
       <c r="H2">
         <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+      <c r="H3">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed drop in button on home to indicate user whether they need to login/signup or if they are already dropped into game
</commit_message>
<xml_diff>
--- a/pyNeedBodies/games.xlsx
+++ b/pyNeedBodies/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>id</t>
   </si>
@@ -49,19 +49,16 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Nic Bolton</t>
   </si>
   <si>
     <t>Prospects Athletics</t>
   </si>
   <si>
-    <t>Atlas Tube Recreation Centre</t>
-  </si>
-  <si>
     <t>nan</t>
+  </si>
+  <si>
+    <t>1;</t>
   </si>
   <si>
     <t>0;</t>
@@ -422,7 +419,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,28 +459,25 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C2">
         <v>20230906</v>
       </c>
       <c r="D2">
-        <v>1000</v>
+        <v>1100</v>
       </c>
       <c r="E2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F2">
         <v>5</v>
       </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H2">
         <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -491,56 +485,27 @@
         <v>10</v>
       </c>
       <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3">
+        <v>20230907</v>
+      </c>
+      <c r="D3">
+        <v>1100</v>
+      </c>
+      <c r="E3" t="s">
         <v>12</v>
       </c>
-      <c r="C3">
-        <v>20230908</v>
-      </c>
-      <c r="D3">
-        <v>2000</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
         <v>14</v>
-      </c>
-      <c r="F3">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>16</v>
       </c>
       <c r="H3">
         <v>2</v>
       </c>
       <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>20231010</v>
-      </c>
-      <c r="D4">
-        <v>900</v>
-      </c>
-      <c r="E4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4">
-        <v>5</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added hashing for passwords!!!
</commit_message>
<xml_diff>
--- a/pyNeedBodies/games.xlsx
+++ b/pyNeedBodies/games.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>id</t>
   </si>
@@ -46,25 +46,16 @@
     <t>0</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>Nic Bolton</t>
   </si>
   <si>
+    <t>20230906</t>
+  </si>
+  <si>
+    <t>0900</t>
+  </si>
+  <si>
     <t>Prospects Athletics</t>
-  </si>
-  <si>
-    <t>Atlas Tube Recreation Centre</t>
-  </si>
-  <si>
-    <t>nan</t>
-  </si>
-  <si>
-    <t>0;</t>
   </si>
 </sst>
 </file>
@@ -422,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I4"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -462,13 +453,13 @@
         <v>9</v>
       </c>
       <c r="B2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="C2">
-        <v>20230906</v>
-      </c>
-      <c r="D2">
-        <v>1100</v>
       </c>
       <c r="E2" t="s">
         <v>13</v>
@@ -476,72 +467,8 @@
       <c r="F2">
         <v>4</v>
       </c>
-      <c r="G2" t="s">
-        <v>15</v>
-      </c>
       <c r="H2">
         <v>2</v>
-      </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>20230907</v>
-      </c>
-      <c r="D3">
-        <v>900</v>
-      </c>
-      <c r="E3" t="s">
-        <v>14</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3">
-        <v>2</v>
-      </c>
-      <c r="I3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4">
-        <v>20230912</v>
-      </c>
-      <c r="D4">
-        <v>900</v>
-      </c>
-      <c r="E4" t="s">
-        <v>14</v>
-      </c>
-      <c r="F4">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
-      </c>
-      <c r="H4">
-        <v>2</v>
-      </c>
-      <c r="I4" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>